<commit_message>
update for error calculation
</commit_message>
<xml_diff>
--- a/Crank-Nicholson Error Calculation.xlsx
+++ b/Crank-Nicholson Error Calculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khale\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0000A22-20B4-4324-80F9-068B378EDBBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C7823B-79B5-4E31-89C1-CDEB35381467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{19DEED89-780B-4EC5-ADD1-99E5A7E37FA5}"/>
   </bookViews>
@@ -77,7 +77,7 @@
     <t>Average Error</t>
   </si>
   <si>
-    <t>Error Calculation for Crank-Nicholson at time = 57.9 days</t>
+    <t xml:space="preserve">Error Calculation for Crank-Nicholson </t>
   </si>
 </sst>
 </file>
@@ -158,10 +158,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -501,7 +501,7 @@
   <dimension ref="A1:Q104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P110" sqref="P110"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,25 +522,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
     </row>
     <row r="2" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -4725,10 +4725,10 @@
       </c>
     </row>
     <row r="104" spans="1:17" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="M104" s="6" t="s">
+      <c r="M104" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N104" s="6"/>
+      <c r="N104" s="5"/>
       <c r="O104" s="3">
         <f>AVERAGE(O3:O103)</f>
         <v>2.3761807920792072E-3</v>

</xml_diff>